<commit_message>
Adding notebooks to new branch
</commit_message>
<xml_diff>
--- a/program_costs/NZSCED to SAC.xlsx
+++ b/program_costs/NZSCED to SAC.xlsx
@@ -1,15 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_F25DC773A252ABEACE02EC0B1B584FE25BDE589D" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{9238B4F2-6FF4-465A-9676-F4288D288B64}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF11E14F-6922-4058-91F2-E1CDDB76FCB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NZSCED to SAC codes" sheetId="1" r:id="rId1"/>
-    <sheet name="NZSCED to SAC costs (2)" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="138">
   <si>
     <t>NZSCED to SAC: SAC category and level</t>
   </si>
@@ -897,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,1721 +2606,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F2AA8F-E63A-452B-8F99-FCD1AADEDAB7}">
-  <dimension ref="A1:G80"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E40" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E42" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E43" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E44" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E46" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E50" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F58" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G58" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="B60" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G60" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G61" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D62" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G63" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G65" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D66" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G67" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D68" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G68" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D70" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G70" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D71" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G71" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D73" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B74" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D74" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C75" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D75" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B76" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C79" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D80" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F80" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010019EDA2D182A5CB4FB9BA8D9AF5786416" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4fd60931bb43e4a6618dcb8ade727f00">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="df735e53-efbe-41fc-ae6f-05ad6d4f423e" xmlns:ns3="5bca14c9-f708-4595-b87f-a3bf9dbbf6b5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9ac9ad4176377412057486f54fcc4f5d" ns2:_="" ns3:_="">
     <xsd:import namespace="df735e53-efbe-41fc-ae6f-05ad6d4f423e"/>
@@ -4538,29 +2838,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA8F37B6-C068-4106-B307-823D4EA44386}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEA07684-1660-413F-AF69-091A0904EA28}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B671D598-BAF3-4416-AF52-8B9C2281CDDC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B671D598-BAF3-4416-AF52-8B9C2281CDDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BEA07684-1660-413F-AF69-091A0904EA28}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA8F37B6-C068-4106-B307-823D4EA44386}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="df735e53-efbe-41fc-ae6f-05ad6d4f423e"/>
+    <ds:schemaRef ds:uri="5bca14c9-f708-4595-b87f-a3bf9dbbf6b5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>